<commit_message>
Modifies hydgn input files to change thermochemical water splitting to POx production
</commit_message>
<xml_diff>
--- a/InputData/hydgn/HPEC/Hydrogen Production Eqpt Costs.xlsx
+++ b/InputData/hydgn/HPEC/Hydrogen Production Eqpt Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\hydgn\HPEC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\hydgn\HPEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144CF766-F142-4FDB-B3C8-5736800C38EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06FFE47-8401-4153-B365-3B8D108180A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30315" yWindow="315" windowWidth="21630" windowHeight="13245" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -125,9 +125,6 @@
     <t>biomass gasification</t>
   </si>
   <si>
-    <t>thermochemical water splitting</t>
-  </si>
-  <si>
     <t>hours per year</t>
   </si>
   <si>
@@ -188,27 +185,6 @@
     <t>Page 7, Table 3</t>
   </si>
   <si>
-    <t>Thermochemical Water Splitting</t>
-  </si>
-  <si>
-    <t>This technology can utilize heat from solar thermal (e.g. mirror</t>
-  </si>
-  <si>
-    <t>collectors, etc.) or from nuclear plants.  Capital costs would</t>
-  </si>
-  <si>
-    <t>vary greatly depending on the technology used.</t>
-  </si>
-  <si>
-    <t>This technology isn't used in the U.S. version of the model,</t>
-  </si>
-  <si>
-    <t>is available for EPS adaptations for other regions or future</t>
-  </si>
-  <si>
-    <t>U.S. region dataset updates.</t>
-  </si>
-  <si>
     <t>2018 USD/2012 USD</t>
   </si>
   <si>
@@ -222,9 +198,6 @@
   </si>
   <si>
     <t>HPEC Hydrogen Production Equipment OpEx</t>
-  </si>
-  <si>
-    <t>so no costs are included here, but the subscript element</t>
   </si>
   <si>
     <t>In other words, this variable should contain the CapEx</t>
@@ -290,6 +263,33 @@
   </si>
   <si>
     <t>natural gas reforming with CCS</t>
+  </si>
+  <si>
+    <t>hydrocarbon partial oxidation</t>
+  </si>
+  <si>
+    <t>Partial Oxidation of Hydrocarbons</t>
+  </si>
+  <si>
+    <t>According to ICF, POx reactors are essentially equivalent to autothermal</t>
+  </si>
+  <si>
+    <t>reformers (ATRs) but without a catalyst bed. For lack of economic data,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">we assume that the costs mirror those of ATRs, which, per ICF, </t>
+  </si>
+  <si>
+    <t>Robertson, Penshorn, and McCurdy</t>
+  </si>
+  <si>
+    <t>Comparing the costs of industrial hydrogen technologies</t>
+  </si>
+  <si>
+    <t>https://www.icf.com/insights/energy/comparing-costs-of-industrial-hydrogen-technologies</t>
+  </si>
+  <si>
+    <t>have ~15% lower capital costs and ~5% lower production costs than SMRs.</t>
   </si>
 </sst>
 </file>
@@ -679,28 +679,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="2" max="2" width="45.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -708,233 +708,239 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="7">
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B37" s="7">
         <v>2014</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B39" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="8" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B48" s="7">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B50" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B39" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B50" r:id="rId3" xr:uid="{0EAF8239-1601-435F-A7F3-DCBE0357401E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -944,15 +950,15 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="1" max="3" width="25.453125" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -972,7 +978,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -992,7 +998,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -1009,7 +1015,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -1026,7 +1032,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="6"/>
       <c r="B5" s="6" t="s">
         <v>14</v>
@@ -1044,7 +1050,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1064,7 +1070,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -1081,7 +1087,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -1098,7 +1104,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="6"/>
       <c r="B9" s="6" t="s">
         <v>17</v>
@@ -1116,7 +1122,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1136,7 +1142,7 @@
         <v>2670</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -1153,7 +1159,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -1170,7 +1176,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="6"/>
       <c r="B13" s="6" t="s">
         <v>17</v>
@@ -1188,8 +1194,8 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1212,33 +1218,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1">
         <f>24*365</f>
         <v>8760</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3412.14</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.91400000000000003</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1253,18 +1261,18 @@
   </sheetPr>
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B1" s="9">
         <v>2017</v>
@@ -1369,7 +1377,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1510,7 +1518,7 @@
         <v>1.3760295531402741E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1651,7 +1659,7 @@
         <v>2.7826375407947768E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1792,7 +1800,7 @@
         <v>8.1644420152989595E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1933,149 +1941,150 @@
         <v>8.1644420152989595E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="B6" s="11">
+        <f>B3*0.85</f>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:R6" si="20">$B6</f>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="D6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="E6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="F6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="G6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="H6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="I6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="J6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="K6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="L6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="M6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="N6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="O6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="P6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="Q6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="R6">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="S6">
         <f t="shared" ref="S6:AI6" si="21">$B6</f>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="T6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="U6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="V6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="W6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="X6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="Y6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="Z6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AA6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AB6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AC6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AD6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AE6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AF6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AG6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AH6">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.3652419096755601E-5</v>
       </c>
       <c r="AI6">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+        <v>2.3652419096755601E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B7" s="11">
         <f>B2</f>
@@ -2214,9 +2223,9 @@
         <v>1.3760295531402741E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B8" s="11">
         <f>B3</f>
@@ -2367,18 +2376,18 @@
   </sheetPr>
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:AI8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B1" s="9">
         <v>2017</v>
@@ -2483,7 +2492,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2624,7 +2633,7 @@
         <v>2.0640443297104109E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2765,7 +2774,7 @@
         <v>1.307839644173545E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2906,7 +2915,7 @@
         <v>4.0822210076494796E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -3047,149 +3056,150 @@
         <v>4.0822210076494796E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="B6" s="11">
+        <f>B3*0.95</f>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:AI6" si="1">$B6</f>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="J6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="L6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="M6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="N6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="O6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="P6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="Q6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="R6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="S6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="T6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="U6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="V6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="W6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="X6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="Y6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="Z6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AA6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AB6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AC6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AD6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AE6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AF6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AG6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AH6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2424476619648677E-6</v>
       </c>
       <c r="AI6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+        <v>1.2424476619648677E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B7" s="11">
         <f>B2</f>
@@ -3328,9 +3338,9 @@
         <v>2.0640443297104109E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B8" s="11">
         <f>B3</f>

</xml_diff>